<commit_message>
elo rating code + the incredible hulk dataset
</commit_message>
<xml_diff>
--- a/Avengers.xlsx
+++ b/Avengers.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Proprietario\Desktop\avengers ELO rating\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Proprietario\Desktop\codici git\avengers ELO rating\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95A2253-76CC-46DC-9CC1-104E56897DCD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA22362-C85F-42EE-B2AB-EB32E966FDDE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{615A6A59-B40D-4CD6-BA71-120B63914EEB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{615A6A59-B40D-4CD6-BA71-120B63914EEB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Iron Man" sheetId="1" r:id="rId1"/>
-    <sheet name="Iron Man 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Captain America" sheetId="3" r:id="rId3"/>
+    <sheet name="Captain America" sheetId="3" r:id="rId1"/>
+    <sheet name="Iron Man" sheetId="1" r:id="rId2"/>
+    <sheet name="L'incredibile Hulk" sheetId="4" r:id="rId3"/>
+    <sheet name="Iron Man 2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="159">
   <si>
     <t>winner</t>
   </si>
@@ -350,9 +351,6 @@
     <t>9-US Army Soldier</t>
   </si>
   <si>
-    <t>50-US Army Soldier</t>
-  </si>
-  <si>
     <t>attacco base principale hydra - arrivo rinforzi</t>
   </si>
   <si>
@@ -362,9 +360,6 @@
     <t>1-Hydra Tank</t>
   </si>
   <si>
-    <t>?-US Army Soldier,Captain America</t>
-  </si>
-  <si>
     <t>scontro finale aereo</t>
   </si>
   <si>
@@ -378,6 +373,144 @@
   </si>
   <si>
     <t>10-terrorist</t>
+  </si>
+  <si>
+    <t>Hulk</t>
+  </si>
+  <si>
+    <t>scena iniziale - esperimento</t>
+  </si>
+  <si>
+    <t>Betty Ross</t>
+  </si>
+  <si>
+    <t>General Ross</t>
+  </si>
+  <si>
+    <t>2-armed civilian</t>
+  </si>
+  <si>
+    <t>(scena solo descritta da Ross)</t>
+  </si>
+  <si>
+    <t>2-civilian</t>
+  </si>
+  <si>
+    <t>?-US Army Soldier WW2,Captain America</t>
+  </si>
+  <si>
+    <t>50-US Army Soldier WW2</t>
+  </si>
+  <si>
+    <t>1-US Army Soldier WW2</t>
+  </si>
+  <si>
+    <t>Emil Blomsky</t>
+  </si>
+  <si>
+    <t>1-dog</t>
+  </si>
+  <si>
+    <t>tentativo di cattura Brasile - casa di Bruce Banner</t>
+  </si>
+  <si>
+    <t>Bruce Banner</t>
+  </si>
+  <si>
+    <t>2-US Army Soldier</t>
+  </si>
+  <si>
+    <t>tentativo di cattura Brasile -fabbrica banner normale</t>
+  </si>
+  <si>
+    <t>tentativo di cattura Brasile -fabbrica trasformazione in hulk</t>
+  </si>
+  <si>
+    <t>battaglia università - prima della trasformazione</t>
+  </si>
+  <si>
+    <t>50 caliber jeep</t>
+  </si>
+  <si>
+    <t>5-Us Army Soldier</t>
+  </si>
+  <si>
+    <t>0.1-Hulk</t>
+  </si>
+  <si>
+    <t>5-Us Army Soldier, 50 caliber jeep</t>
+  </si>
+  <si>
+    <t>0.2-Hulk</t>
+  </si>
+  <si>
+    <t>8-Us Army Soldier</t>
+  </si>
+  <si>
+    <t>0.5-Hulk</t>
+  </si>
+  <si>
+    <t>2-Sonic weapon jeep</t>
+  </si>
+  <si>
+    <t>Sonic weapon jeep</t>
+  </si>
+  <si>
+    <t>1-Assault Chopper</t>
+  </si>
+  <si>
+    <t>battaglia università - hulk vs fanteria</t>
+  </si>
+  <si>
+    <t>battaglia università - hulk vs blomsky e jeep sperimentali</t>
+  </si>
+  <si>
+    <t>battaglia università - hulk vs elicottero</t>
+  </si>
+  <si>
+    <t>battaglia finale città - laboratorio di Samuel Sterns</t>
+  </si>
+  <si>
+    <t>Samuel Sterns</t>
+  </si>
+  <si>
+    <t>battaglia finale città - nascita di Abominio</t>
+  </si>
+  <si>
+    <t>Abominio</t>
+  </si>
+  <si>
+    <t>1-car</t>
+  </si>
+  <si>
+    <t>?-car</t>
+  </si>
+  <si>
+    <t>?-US Army Soldier</t>
+  </si>
+  <si>
+    <t>?-policeman</t>
+  </si>
+  <si>
+    <t>6-policeman</t>
+  </si>
+  <si>
+    <t>11-car</t>
+  </si>
+  <si>
+    <t>battaglia finale città - Abominio fa casino</t>
+  </si>
+  <si>
+    <t>0.1-Abominio</t>
+  </si>
+  <si>
+    <t>1-Chopper w Minigun</t>
+  </si>
+  <si>
+    <t>battaglia finale città - Hulk vs Abominio (strade)</t>
+  </si>
+  <si>
+    <t>battaglia finale città - Hulk vs Abominio (tetto)</t>
   </si>
 </sst>
 </file>
@@ -736,11 +869,832 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A0F2A9D-6D91-4F82-87B0-BEB6D55B1196}">
+  <dimension ref="A1:E47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.88671875" customWidth="1"/>
+    <col min="2" max="2" width="22.77734375" customWidth="1"/>
+    <col min="3" max="3" width="41.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.21875" customWidth="1"/>
+    <col min="5" max="5" width="23.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" t="s">
+        <v>94</v>
+      </c>
+      <c r="D26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" t="s">
+        <v>100</v>
+      </c>
+      <c r="D30" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>102</v>
+      </c>
+      <c r="B31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" t="s">
+        <v>100</v>
+      </c>
+      <c r="D31" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" t="s">
+        <v>101</v>
+      </c>
+      <c r="C32" t="s">
+        <v>105</v>
+      </c>
+      <c r="D32" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>103</v>
+      </c>
+      <c r="B34" t="s">
+        <v>104</v>
+      </c>
+      <c r="C34" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>121</v>
+      </c>
+      <c r="B35" t="s">
+        <v>106</v>
+      </c>
+      <c r="C35" t="s">
+        <v>105</v>
+      </c>
+      <c r="D35" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" t="s">
+        <v>105</v>
+      </c>
+      <c r="D36" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37" t="s">
+        <v>105</v>
+      </c>
+      <c r="D37" t="s">
+        <v>33</v>
+      </c>
+      <c r="E37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" t="s">
+        <v>105</v>
+      </c>
+      <c r="D38" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>120</v>
+      </c>
+      <c r="B39" t="s">
+        <v>85</v>
+      </c>
+      <c r="C39" t="s">
+        <v>105</v>
+      </c>
+      <c r="D39" t="s">
+        <v>33</v>
+      </c>
+      <c r="E39" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>88</v>
+      </c>
+      <c r="B40" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" t="s">
+        <v>105</v>
+      </c>
+      <c r="D40" t="s">
+        <v>33</v>
+      </c>
+      <c r="E40" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" t="s">
+        <v>109</v>
+      </c>
+      <c r="C41" t="s">
+        <v>108</v>
+      </c>
+      <c r="D41" t="s">
+        <v>33</v>
+      </c>
+      <c r="E41" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" t="s">
+        <v>77</v>
+      </c>
+      <c r="C42" t="s">
+        <v>108</v>
+      </c>
+      <c r="D42" t="s">
+        <v>34</v>
+      </c>
+      <c r="E42" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" t="s">
+        <v>108</v>
+      </c>
+      <c r="D43" t="s">
+        <v>33</v>
+      </c>
+      <c r="E43" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" t="s">
+        <v>108</v>
+      </c>
+      <c r="D44" t="s">
+        <v>33</v>
+      </c>
+      <c r="E44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>72</v>
+      </c>
+      <c r="B45" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" t="s">
+        <v>108</v>
+      </c>
+      <c r="D45" t="s">
+        <v>33</v>
+      </c>
+      <c r="E45" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>80</v>
+      </c>
+      <c r="B46" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46" t="s">
+        <v>108</v>
+      </c>
+      <c r="D46" t="s">
+        <v>33</v>
+      </c>
+      <c r="E46" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>80</v>
+      </c>
+      <c r="B47" t="s">
+        <v>110</v>
+      </c>
+      <c r="C47" t="s">
+        <v>111</v>
+      </c>
+      <c r="D47" t="s">
+        <v>33</v>
+      </c>
+      <c r="E47" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FDFF9AB-D405-44AD-BBAB-3BB81B18670C}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -825,7 +1779,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -1255,7 +2209,1135 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A6E19BE-BCA4-4601-93CD-8C178C0CE457}">
+  <dimension ref="A1:E65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34.109375" customWidth="1"/>
+    <col min="2" max="2" width="38" customWidth="1"/>
+    <col min="3" max="3" width="64.77734375" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>128</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>129</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>113</v>
+      </c>
+      <c r="B14" t="s">
+        <v>127</v>
+      </c>
+      <c r="C14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C15" t="s">
+        <v>129</v>
+      </c>
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16" t="s">
+        <v>129</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" t="s">
+        <v>130</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" t="s">
+        <v>115</v>
+      </c>
+      <c r="C18" t="s">
+        <v>130</v>
+      </c>
+      <c r="D18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>132</v>
+      </c>
+      <c r="B19" t="s">
+        <v>133</v>
+      </c>
+      <c r="C19" t="s">
+        <v>141</v>
+      </c>
+      <c r="D19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>134</v>
+      </c>
+      <c r="B20" t="s">
+        <v>135</v>
+      </c>
+      <c r="C20" t="s">
+        <v>141</v>
+      </c>
+      <c r="D20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21" t="s">
+        <v>141</v>
+      </c>
+      <c r="D21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" t="s">
+        <v>131</v>
+      </c>
+      <c r="C22" t="s">
+        <v>141</v>
+      </c>
+      <c r="D22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>113</v>
+      </c>
+      <c r="B23" t="s">
+        <v>136</v>
+      </c>
+      <c r="C23" t="s">
+        <v>141</v>
+      </c>
+      <c r="D23" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" t="s">
+        <v>141</v>
+      </c>
+      <c r="D24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" t="s">
+        <v>137</v>
+      </c>
+      <c r="C25" t="s">
+        <v>142</v>
+      </c>
+      <c r="D25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>123</v>
+      </c>
+      <c r="B26" t="s">
+        <v>135</v>
+      </c>
+      <c r="C26" t="s">
+        <v>142</v>
+      </c>
+      <c r="D26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>123</v>
+      </c>
+      <c r="B27" t="s">
+        <v>133</v>
+      </c>
+      <c r="C27" t="s">
+        <v>142</v>
+      </c>
+      <c r="D27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>138</v>
+      </c>
+      <c r="B28" t="s">
+        <v>123</v>
+      </c>
+      <c r="C28" t="s">
+        <v>142</v>
+      </c>
+      <c r="D28" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>138</v>
+      </c>
+      <c r="B29" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29" t="s">
+        <v>142</v>
+      </c>
+      <c r="D29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>113</v>
+      </c>
+      <c r="B30" t="s">
+        <v>139</v>
+      </c>
+      <c r="C30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D30" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" t="s">
+        <v>139</v>
+      </c>
+      <c r="C31" t="s">
+        <v>142</v>
+      </c>
+      <c r="D31" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>113</v>
+      </c>
+      <c r="B32" t="s">
+        <v>123</v>
+      </c>
+      <c r="C32" t="s">
+        <v>142</v>
+      </c>
+      <c r="D32" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>140</v>
+      </c>
+      <c r="B33" t="s">
+        <v>135</v>
+      </c>
+      <c r="C33" t="s">
+        <v>143</v>
+      </c>
+      <c r="D33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>113</v>
+      </c>
+      <c r="B34" t="s">
+        <v>140</v>
+      </c>
+      <c r="C34" t="s">
+        <v>143</v>
+      </c>
+      <c r="D34" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" t="s">
+        <v>126</v>
+      </c>
+      <c r="C35" t="s">
+        <v>144</v>
+      </c>
+      <c r="D35" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>123</v>
+      </c>
+      <c r="B36" t="s">
+        <v>115</v>
+      </c>
+      <c r="C36" t="s">
+        <v>144</v>
+      </c>
+      <c r="D36" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>123</v>
+      </c>
+      <c r="B37" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" t="s">
+        <v>146</v>
+      </c>
+      <c r="D37" t="s">
+        <v>33</v>
+      </c>
+      <c r="E37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>123</v>
+      </c>
+      <c r="B38" t="s">
+        <v>145</v>
+      </c>
+      <c r="C38" t="s">
+        <v>146</v>
+      </c>
+      <c r="D38" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>147</v>
+      </c>
+      <c r="B39" t="s">
+        <v>145</v>
+      </c>
+      <c r="C39" t="s">
+        <v>146</v>
+      </c>
+      <c r="D39" t="s">
+        <v>33</v>
+      </c>
+      <c r="E39" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>147</v>
+      </c>
+      <c r="B40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" t="s">
+        <v>146</v>
+      </c>
+      <c r="D40" t="s">
+        <v>33</v>
+      </c>
+      <c r="E40" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>147</v>
+      </c>
+      <c r="B41" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" t="s">
+        <v>146</v>
+      </c>
+      <c r="D41" t="s">
+        <v>33</v>
+      </c>
+      <c r="E41" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>147</v>
+      </c>
+      <c r="B42" t="s">
+        <v>148</v>
+      </c>
+      <c r="C42" t="s">
+        <v>154</v>
+      </c>
+      <c r="D42" t="s">
+        <v>33</v>
+      </c>
+      <c r="E42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>147</v>
+      </c>
+      <c r="B43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" t="s">
+        <v>154</v>
+      </c>
+      <c r="D43" t="s">
+        <v>33</v>
+      </c>
+      <c r="E43" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>147</v>
+      </c>
+      <c r="B44" t="s">
+        <v>148</v>
+      </c>
+      <c r="C44" t="s">
+        <v>154</v>
+      </c>
+      <c r="D44" t="s">
+        <v>33</v>
+      </c>
+      <c r="E44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>147</v>
+      </c>
+      <c r="B45" t="s">
+        <v>149</v>
+      </c>
+      <c r="C45" t="s">
+        <v>154</v>
+      </c>
+      <c r="D45" t="s">
+        <v>33</v>
+      </c>
+      <c r="E45" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>147</v>
+      </c>
+      <c r="B46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" t="s">
+        <v>154</v>
+      </c>
+      <c r="D46" t="s">
+        <v>33</v>
+      </c>
+      <c r="E46" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>147</v>
+      </c>
+      <c r="B47" t="s">
+        <v>150</v>
+      </c>
+      <c r="C47" t="s">
+        <v>154</v>
+      </c>
+      <c r="D47" t="s">
+        <v>33</v>
+      </c>
+      <c r="E47" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>147</v>
+      </c>
+      <c r="B48" t="s">
+        <v>151</v>
+      </c>
+      <c r="C48" t="s">
+        <v>154</v>
+      </c>
+      <c r="D48" t="s">
+        <v>33</v>
+      </c>
+      <c r="E48" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>147</v>
+      </c>
+      <c r="B49" t="s">
+        <v>20</v>
+      </c>
+      <c r="C49" t="s">
+        <v>154</v>
+      </c>
+      <c r="D49" t="s">
+        <v>33</v>
+      </c>
+      <c r="E49" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>147</v>
+      </c>
+      <c r="B50" t="s">
+        <v>152</v>
+      </c>
+      <c r="C50" t="s">
+        <v>154</v>
+      </c>
+      <c r="D50" t="s">
+        <v>33</v>
+      </c>
+      <c r="E50" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>147</v>
+      </c>
+      <c r="B51" t="s">
+        <v>153</v>
+      </c>
+      <c r="C51" t="s">
+        <v>154</v>
+      </c>
+      <c r="D51" t="s">
+        <v>33</v>
+      </c>
+      <c r="E51" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>147</v>
+      </c>
+      <c r="B52" t="s">
+        <v>71</v>
+      </c>
+      <c r="C52" t="s">
+        <v>154</v>
+      </c>
+      <c r="D52" t="s">
+        <v>33</v>
+      </c>
+      <c r="E52" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>147</v>
+      </c>
+      <c r="B53" t="s">
+        <v>46</v>
+      </c>
+      <c r="C53" t="s">
+        <v>154</v>
+      </c>
+      <c r="D53" t="s">
+        <v>33</v>
+      </c>
+      <c r="E53" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>147</v>
+      </c>
+      <c r="B54" t="s">
+        <v>19</v>
+      </c>
+      <c r="C54" t="s">
+        <v>157</v>
+      </c>
+      <c r="D54" t="s">
+        <v>33</v>
+      </c>
+      <c r="E54" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>147</v>
+      </c>
+      <c r="B55" t="s">
+        <v>113</v>
+      </c>
+      <c r="C55" t="s">
+        <v>157</v>
+      </c>
+      <c r="D55" t="s">
+        <v>33</v>
+      </c>
+      <c r="E55" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>113</v>
+      </c>
+      <c r="B56" t="s">
+        <v>148</v>
+      </c>
+      <c r="C56" t="s">
+        <v>157</v>
+      </c>
+      <c r="D56" t="s">
+        <v>33</v>
+      </c>
+      <c r="E56" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>113</v>
+      </c>
+      <c r="B57" t="s">
+        <v>147</v>
+      </c>
+      <c r="C57" t="s">
+        <v>157</v>
+      </c>
+      <c r="D57" t="s">
+        <v>33</v>
+      </c>
+      <c r="E57" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>147</v>
+      </c>
+      <c r="B58" t="s">
+        <v>113</v>
+      </c>
+      <c r="C58" t="s">
+        <v>157</v>
+      </c>
+      <c r="D58" t="s">
+        <v>33</v>
+      </c>
+      <c r="E58" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>156</v>
+      </c>
+      <c r="B59" t="s">
+        <v>155</v>
+      </c>
+      <c r="C59" t="s">
+        <v>157</v>
+      </c>
+      <c r="D59" t="s">
+        <v>34</v>
+      </c>
+      <c r="E59" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>147</v>
+      </c>
+      <c r="B60" t="s">
+        <v>156</v>
+      </c>
+      <c r="C60" t="s">
+        <v>157</v>
+      </c>
+      <c r="D60" t="s">
+        <v>34</v>
+      </c>
+      <c r="E60" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>147</v>
+      </c>
+      <c r="B61" t="s">
+        <v>137</v>
+      </c>
+      <c r="C61" t="s">
+        <v>158</v>
+      </c>
+      <c r="D61" t="s">
+        <v>33</v>
+      </c>
+      <c r="E61" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>113</v>
+      </c>
+      <c r="B62" t="s">
+        <v>147</v>
+      </c>
+      <c r="C62" t="s">
+        <v>158</v>
+      </c>
+      <c r="D62" t="s">
+        <v>33</v>
+      </c>
+      <c r="E62" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>147</v>
+      </c>
+      <c r="B63" t="s">
+        <v>113</v>
+      </c>
+      <c r="C63" t="s">
+        <v>158</v>
+      </c>
+      <c r="D63" t="s">
+        <v>33</v>
+      </c>
+      <c r="E63" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>147</v>
+      </c>
+      <c r="B64" t="s">
+        <v>113</v>
+      </c>
+      <c r="C64" t="s">
+        <v>158</v>
+      </c>
+      <c r="D64" t="s">
+        <v>33</v>
+      </c>
+      <c r="E64" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>113</v>
+      </c>
+      <c r="B65" t="s">
+        <v>147</v>
+      </c>
+      <c r="C65" t="s">
+        <v>158</v>
+      </c>
+      <c r="D65" t="s">
+        <v>33</v>
+      </c>
+      <c r="E65" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97203B1C-8A29-4438-986F-111AFC7E55B4}">
   <dimension ref="A1:E26"/>
   <sheetViews>
@@ -1717,825 +3799,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A0F2A9D-6D91-4F82-87B0-BEB6D55B1196}">
-  <dimension ref="A1:E47"/>
-  <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="32.88671875" customWidth="1"/>
-    <col min="2" max="2" width="22.77734375" customWidth="1"/>
-    <col min="3" max="3" width="41.6640625" customWidth="1"/>
-    <col min="4" max="4" width="23.21875" customWidth="1"/>
-    <col min="5" max="5" width="23.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B8" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B9" t="s">
-        <v>77</v>
-      </c>
-      <c r="C9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B11" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" t="s">
-        <v>84</v>
-      </c>
-      <c r="D11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>86</v>
-      </c>
-      <c r="B12" t="s">
-        <v>87</v>
-      </c>
-      <c r="C12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>80</v>
-      </c>
-      <c r="B13" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>80</v>
-      </c>
-      <c r="B14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" t="s">
-        <v>84</v>
-      </c>
-      <c r="D14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>80</v>
-      </c>
-      <c r="B15" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" t="s">
-        <v>91</v>
-      </c>
-      <c r="D15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>96</v>
-      </c>
-      <c r="B16" t="s">
-        <v>88</v>
-      </c>
-      <c r="C16" t="s">
-        <v>91</v>
-      </c>
-      <c r="D16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>89</v>
-      </c>
-      <c r="B17" t="s">
-        <v>108</v>
-      </c>
-      <c r="C17" t="s">
-        <v>91</v>
-      </c>
-      <c r="D17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" t="s">
-        <v>92</v>
-      </c>
-      <c r="D18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>80</v>
-      </c>
-      <c r="B19" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" t="s">
-        <v>92</v>
-      </c>
-      <c r="D19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>97</v>
-      </c>
-      <c r="B20" t="s">
-        <v>90</v>
-      </c>
-      <c r="C20" t="s">
-        <v>92</v>
-      </c>
-      <c r="D20" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>72</v>
-      </c>
-      <c r="B21" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" t="s">
-        <v>92</v>
-      </c>
-      <c r="D21" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>67</v>
-      </c>
-      <c r="B22" t="s">
-        <v>93</v>
-      </c>
-      <c r="C22" t="s">
-        <v>94</v>
-      </c>
-      <c r="D22" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>80</v>
-      </c>
-      <c r="B23" t="s">
-        <v>77</v>
-      </c>
-      <c r="C23" t="s">
-        <v>94</v>
-      </c>
-      <c r="D23" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>95</v>
-      </c>
-      <c r="B24" t="s">
-        <v>77</v>
-      </c>
-      <c r="C24" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>77</v>
-      </c>
-      <c r="B25" t="s">
-        <v>80</v>
-      </c>
-      <c r="C25" t="s">
-        <v>94</v>
-      </c>
-      <c r="D25" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" t="s">
-        <v>94</v>
-      </c>
-      <c r="D26" t="s">
-        <v>33</v>
-      </c>
-      <c r="E26" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>80</v>
-      </c>
-      <c r="B27" t="s">
-        <v>77</v>
-      </c>
-      <c r="C27" t="s">
-        <v>94</v>
-      </c>
-      <c r="D27" t="s">
-        <v>33</v>
-      </c>
-      <c r="E27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>89</v>
-      </c>
-      <c r="B28" t="s">
-        <v>98</v>
-      </c>
-      <c r="C28" t="s">
-        <v>94</v>
-      </c>
-      <c r="D28" t="s">
-        <v>33</v>
-      </c>
-      <c r="E28" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>89</v>
-      </c>
-      <c r="B29" t="s">
-        <v>77</v>
-      </c>
-      <c r="C29" t="s">
-        <v>94</v>
-      </c>
-      <c r="D29" t="s">
-        <v>33</v>
-      </c>
-      <c r="E29" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>80</v>
-      </c>
-      <c r="B30" t="s">
-        <v>99</v>
-      </c>
-      <c r="C30" t="s">
-        <v>100</v>
-      </c>
-      <c r="D30" t="s">
-        <v>33</v>
-      </c>
-      <c r="E30" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>102</v>
-      </c>
-      <c r="B31" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" t="s">
-        <v>100</v>
-      </c>
-      <c r="D31" t="s">
-        <v>33</v>
-      </c>
-      <c r="E31" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>97</v>
-      </c>
-      <c r="B32" t="s">
-        <v>101</v>
-      </c>
-      <c r="C32" t="s">
-        <v>106</v>
-      </c>
-      <c r="D32" t="s">
-        <v>33</v>
-      </c>
-      <c r="E32" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>89</v>
-      </c>
-      <c r="B33" t="s">
-        <v>93</v>
-      </c>
-      <c r="C33" t="s">
-        <v>106</v>
-      </c>
-      <c r="D33" t="s">
-        <v>33</v>
-      </c>
-      <c r="E33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>103</v>
-      </c>
-      <c r="B34" t="s">
-        <v>104</v>
-      </c>
-      <c r="C34" t="s">
-        <v>106</v>
-      </c>
-      <c r="D34" t="s">
-        <v>33</v>
-      </c>
-      <c r="E34" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>105</v>
-      </c>
-      <c r="B35" t="s">
-        <v>107</v>
-      </c>
-      <c r="C35" t="s">
-        <v>106</v>
-      </c>
-      <c r="D35" t="s">
-        <v>33</v>
-      </c>
-      <c r="E35" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>72</v>
-      </c>
-      <c r="B36" t="s">
-        <v>71</v>
-      </c>
-      <c r="C36" t="s">
-        <v>106</v>
-      </c>
-      <c r="D36" t="s">
-        <v>33</v>
-      </c>
-      <c r="E36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37" t="s">
-        <v>83</v>
-      </c>
-      <c r="C37" t="s">
-        <v>106</v>
-      </c>
-      <c r="D37" t="s">
-        <v>33</v>
-      </c>
-      <c r="E37" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>79</v>
-      </c>
-      <c r="B38" t="s">
-        <v>77</v>
-      </c>
-      <c r="C38" t="s">
-        <v>106</v>
-      </c>
-      <c r="D38" t="s">
-        <v>33</v>
-      </c>
-      <c r="E38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>109</v>
-      </c>
-      <c r="B39" t="s">
-        <v>85</v>
-      </c>
-      <c r="C39" t="s">
-        <v>106</v>
-      </c>
-      <c r="D39" t="s">
-        <v>33</v>
-      </c>
-      <c r="E39" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>88</v>
-      </c>
-      <c r="B40" t="s">
-        <v>71</v>
-      </c>
-      <c r="C40" t="s">
-        <v>106</v>
-      </c>
-      <c r="D40" t="s">
-        <v>33</v>
-      </c>
-      <c r="E40" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>80</v>
-      </c>
-      <c r="B41" t="s">
-        <v>111</v>
-      </c>
-      <c r="C41" t="s">
-        <v>110</v>
-      </c>
-      <c r="D41" t="s">
-        <v>33</v>
-      </c>
-      <c r="E41" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>80</v>
-      </c>
-      <c r="B42" t="s">
-        <v>77</v>
-      </c>
-      <c r="C42" t="s">
-        <v>110</v>
-      </c>
-      <c r="D42" t="s">
-        <v>34</v>
-      </c>
-      <c r="E42" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>72</v>
-      </c>
-      <c r="B43" t="s">
-        <v>80</v>
-      </c>
-      <c r="C43" t="s">
-        <v>110</v>
-      </c>
-      <c r="D43" t="s">
-        <v>33</v>
-      </c>
-      <c r="E43" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>80</v>
-      </c>
-      <c r="B44" t="s">
-        <v>72</v>
-      </c>
-      <c r="C44" t="s">
-        <v>110</v>
-      </c>
-      <c r="D44" t="s">
-        <v>33</v>
-      </c>
-      <c r="E44" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>72</v>
-      </c>
-      <c r="B45" t="s">
-        <v>80</v>
-      </c>
-      <c r="C45" t="s">
-        <v>110</v>
-      </c>
-      <c r="D45" t="s">
-        <v>33</v>
-      </c>
-      <c r="E45" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>80</v>
-      </c>
-      <c r="B46" t="s">
-        <v>72</v>
-      </c>
-      <c r="C46" t="s">
-        <v>110</v>
-      </c>
-      <c r="D46" t="s">
-        <v>33</v>
-      </c>
-      <c r="E46" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>80</v>
-      </c>
-      <c r="B47" t="s">
-        <v>112</v>
-      </c>
-      <c r="C47" t="s">
-        <v>113</v>
-      </c>
-      <c r="D47" t="s">
-        <v>33</v>
-      </c>
-      <c r="E47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
shiny app + embetter df
</commit_message>
<xml_diff>
--- a/Avengers.xlsx
+++ b/Avengers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Proprietario\Desktop\codici git\avengers ELO rating\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1D3753-E888-4794-88DD-898C4D1BAB74}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85245FAA-D3EE-4767-8F5B-89D5BCA99954}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" activeTab="4" xr2:uid="{615A6A59-B40D-4CD6-BA71-120B63914EEB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{615A6A59-B40D-4CD6-BA71-120B63914EEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Captain America" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1965" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1965" uniqueCount="289">
   <si>
     <t>winner</t>
   </si>
@@ -804,9 +804,6 @@
   </si>
   <si>
     <t>Battaglia di New York - Thor vs Loki</t>
-  </si>
-  <si>
-    <t>Ironman</t>
   </si>
   <si>
     <t>1-Chitauri Speedbike</t>
@@ -1276,7 +1273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A0F2A9D-6D91-4F82-87B0-BEB6D55B1196}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2097,8 +2094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FDFF9AB-D405-44AD-BBAB-3BB81B18670C}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2634,7 +2631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A6E19BE-BCA4-4601-93CD-8C178C0CE457}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
@@ -3762,7 +3759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86623F91-13E1-4965-971C-80C3CB3164C6}">
   <dimension ref="A1:E90"/>
   <sheetViews>
-    <sheetView topLeftCell="A75" workbookViewId="0">
+    <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -5314,7 +5311,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97203B1C-8A29-4438-986F-111AFC7E55B4}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -5778,8 +5775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21457546-0B28-49FC-B4FE-8AD5E29F1C13}">
   <dimension ref="A1:E135"/>
   <sheetViews>
-    <sheetView topLeftCell="A118" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D134" sqref="D134:E135"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6898,13 +6895,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
+        <v>2</v>
+      </c>
+      <c r="B66" t="s">
         <v>256</v>
       </c>
-      <c r="B66" t="s">
-        <v>257</v>
-      </c>
       <c r="C66" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D66" t="s">
         <v>33</v>
@@ -6915,13 +6912,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
+        <v>257</v>
+      </c>
+      <c r="B67" t="s">
         <v>258</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
         <v>259</v>
-      </c>
-      <c r="C67" t="s">
-        <v>260</v>
       </c>
       <c r="D67" t="s">
         <v>33</v>
@@ -6932,13 +6929,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B68" t="s">
         <v>250</v>
       </c>
       <c r="C68" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D68" t="s">
         <v>33</v>
@@ -6952,7 +6949,7 @@
         <v>176</v>
       </c>
       <c r="B69" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C69" t="s">
         <v>255</v>
@@ -6969,7 +6966,7 @@
         <v>176</v>
       </c>
       <c r="B70" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C70" t="s">
         <v>255</v>
@@ -7000,13 +6997,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B72" t="s">
         <v>18</v>
       </c>
       <c r="C72" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D72" t="s">
         <v>32</v>
@@ -7020,7 +7017,7 @@
         <v>176</v>
       </c>
       <c r="B73" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C73" t="s">
         <v>255</v>
@@ -7051,13 +7048,13 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
+        <v>262</v>
+      </c>
+      <c r="B75" t="s">
         <v>263</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" t="s">
         <v>264</v>
-      </c>
-      <c r="C75" t="s">
-        <v>265</v>
       </c>
       <c r="D75" t="s">
         <v>32</v>
@@ -7068,13 +7065,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B76" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C76" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D76" t="s">
         <v>32</v>
@@ -7088,10 +7085,10 @@
         <v>214</v>
       </c>
       <c r="B77" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C77" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D77" t="s">
         <v>32</v>
@@ -7105,10 +7102,10 @@
         <v>48</v>
       </c>
       <c r="B78" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C78" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D78" t="s">
         <v>32</v>
@@ -7122,10 +7119,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C79" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D79" t="s">
         <v>32</v>
@@ -7139,10 +7136,10 @@
         <v>214</v>
       </c>
       <c r="B80" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C80" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D80" t="s">
         <v>32</v>
@@ -7156,10 +7153,10 @@
         <v>48</v>
       </c>
       <c r="B81" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C81" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D81" t="s">
         <v>32</v>
@@ -7170,13 +7167,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B82" t="s">
         <v>214</v>
       </c>
       <c r="C82" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D82" t="s">
         <v>32</v>
@@ -7190,10 +7187,10 @@
         <v>48</v>
       </c>
       <c r="B83" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C83" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D83" t="s">
         <v>32</v>
@@ -7207,10 +7204,10 @@
         <v>214</v>
       </c>
       <c r="B84" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C84" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D84" t="s">
         <v>32</v>
@@ -7224,10 +7221,10 @@
         <v>214</v>
       </c>
       <c r="B85" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C85" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D85" t="s">
         <v>32</v>
@@ -7241,10 +7238,10 @@
         <v>78</v>
       </c>
       <c r="B86" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C86" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D86" t="s">
         <v>32</v>
@@ -7258,10 +7255,10 @@
         <v>157</v>
       </c>
       <c r="B87" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C87" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D87" t="s">
         <v>33</v>
@@ -7272,13 +7269,13 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
+        <v>269</v>
+      </c>
+      <c r="B88" t="s">
+        <v>268</v>
+      </c>
+      <c r="C88" t="s">
         <v>270</v>
-      </c>
-      <c r="B88" t="s">
-        <v>269</v>
-      </c>
-      <c r="C88" t="s">
-        <v>271</v>
       </c>
       <c r="D88" t="s">
         <v>32</v>
@@ -7292,10 +7289,10 @@
         <v>111</v>
       </c>
       <c r="B89" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C89" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D89" t="s">
         <v>33</v>
@@ -7312,7 +7309,7 @@
         <v>250</v>
       </c>
       <c r="C90" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D90" t="s">
         <v>33</v>
@@ -7329,7 +7326,7 @@
         <v>251</v>
       </c>
       <c r="C91" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D91" t="s">
         <v>32</v>
@@ -7343,10 +7340,10 @@
         <v>157</v>
       </c>
       <c r="B92" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C92" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D92" t="s">
         <v>32</v>
@@ -7363,7 +7360,7 @@
         <v>253</v>
       </c>
       <c r="C93" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D93" t="s">
         <v>32</v>
@@ -7377,10 +7374,10 @@
         <v>2</v>
       </c>
       <c r="B94" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C94" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D94" t="s">
         <v>33</v>
@@ -7397,7 +7394,7 @@
         <v>253</v>
       </c>
       <c r="C95" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D95" t="s">
         <v>33</v>
@@ -7408,13 +7405,13 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B96" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C96" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D96" t="s">
         <v>32</v>
@@ -7428,10 +7425,10 @@
         <v>48</v>
       </c>
       <c r="B97" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C97" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D97" t="s">
         <v>32</v>
@@ -7445,10 +7442,10 @@
         <v>48</v>
       </c>
       <c r="B98" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C98" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D98" t="s">
         <v>33</v>
@@ -7462,10 +7459,10 @@
         <v>2</v>
       </c>
       <c r="B99" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C99" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D99" t="s">
         <v>33</v>
@@ -7479,10 +7476,10 @@
         <v>2</v>
       </c>
       <c r="B100" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C100" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D100" t="s">
         <v>33</v>
@@ -7496,10 +7493,10 @@
         <v>78</v>
       </c>
       <c r="B101" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C101" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D101" t="s">
         <v>32</v>
@@ -7513,10 +7510,10 @@
         <v>2</v>
       </c>
       <c r="B102" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C102" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D102" t="s">
         <v>32</v>
@@ -7527,13 +7524,13 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B103" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C103" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D103" t="s">
         <v>32</v>
@@ -7547,10 +7544,10 @@
         <v>2</v>
       </c>
       <c r="B104" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C104" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D104" t="s">
         <v>33</v>
@@ -7564,10 +7561,10 @@
         <v>214</v>
       </c>
       <c r="B105" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C105" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D105" t="s">
         <v>32</v>
@@ -7581,10 +7578,10 @@
         <v>214</v>
       </c>
       <c r="B106" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C106" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D106" t="s">
         <v>32</v>
@@ -7598,10 +7595,10 @@
         <v>111</v>
       </c>
       <c r="B107" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C107" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D107" t="s">
         <v>32</v>
@@ -7615,10 +7612,10 @@
         <v>157</v>
       </c>
       <c r="B108" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C108" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D108" t="s">
         <v>32</v>
@@ -7629,13 +7626,13 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B109" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C109" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D109" t="s">
         <v>32</v>
@@ -7652,7 +7649,7 @@
         <v>157</v>
       </c>
       <c r="C110" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D110" t="s">
         <v>32</v>
@@ -7663,13 +7660,13 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B111" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C111" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D111" t="s">
         <v>32</v>
@@ -7683,10 +7680,10 @@
         <v>78</v>
       </c>
       <c r="B112" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C112" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D112" t="s">
         <v>32</v>
@@ -7700,10 +7697,10 @@
         <v>78</v>
       </c>
       <c r="B113" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C113" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D113" t="s">
         <v>32</v>
@@ -7714,13 +7711,13 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B114" t="s">
+        <v>277</v>
+      </c>
+      <c r="C114" t="s">
         <v>278</v>
-      </c>
-      <c r="C114" t="s">
-        <v>279</v>
       </c>
       <c r="D114" t="s">
         <v>32</v>
@@ -7734,10 +7731,10 @@
         <v>78</v>
       </c>
       <c r="B115" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C115" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D115" t="s">
         <v>32</v>
@@ -7754,7 +7751,7 @@
         <v>176</v>
       </c>
       <c r="C116" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D116" t="s">
         <v>32</v>
@@ -7768,10 +7765,10 @@
         <v>214</v>
       </c>
       <c r="B117" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C117" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D117" t="s">
         <v>32</v>
@@ -7788,7 +7785,7 @@
         <v>176</v>
       </c>
       <c r="C118" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D118" t="s">
         <v>33</v>
@@ -7805,7 +7802,7 @@
         <v>176</v>
       </c>
       <c r="C119" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D119" t="s">
         <v>32</v>
@@ -7822,7 +7819,7 @@
         <v>176</v>
       </c>
       <c r="C120" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D120" t="s">
         <v>32</v>
@@ -7836,10 +7833,10 @@
         <v>157</v>
       </c>
       <c r="B121" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C121" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D121" t="s">
         <v>33</v>
@@ -7853,10 +7850,10 @@
         <v>157</v>
       </c>
       <c r="B122" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C122" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D122" t="s">
         <v>33</v>
@@ -7870,10 +7867,10 @@
         <v>2</v>
       </c>
       <c r="B123" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C123" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D123" t="s">
         <v>33</v>
@@ -7884,13 +7881,13 @@
     </row>
     <row r="124" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B124" t="s">
         <v>2</v>
       </c>
       <c r="C124" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D124" t="s">
         <v>32</v>
@@ -7904,10 +7901,10 @@
         <v>214</v>
       </c>
       <c r="B125" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C125" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D125" t="s">
         <v>32</v>
@@ -7921,10 +7918,10 @@
         <v>111</v>
       </c>
       <c r="B126" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C126" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D126" t="s">
         <v>32</v>
@@ -7935,13 +7932,13 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
+        <v>281</v>
+      </c>
+      <c r="B127" t="s">
         <v>282</v>
       </c>
-      <c r="B127" t="s">
-        <v>283</v>
-      </c>
       <c r="C127" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D127" t="s">
         <v>33</v>
@@ -7958,7 +7955,7 @@
         <v>238</v>
       </c>
       <c r="C128" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D128" t="s">
         <v>32</v>
@@ -7969,13 +7966,13 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B129" t="s">
         <v>232</v>
       </c>
       <c r="C129" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D129" t="s">
         <v>32</v>
@@ -7989,10 +7986,10 @@
         <v>2</v>
       </c>
       <c r="B130" t="s">
+        <v>283</v>
+      </c>
+      <c r="C130" t="s">
         <v>284</v>
-      </c>
-      <c r="C130" t="s">
-        <v>285</v>
       </c>
       <c r="D130" t="s">
         <v>32</v>
@@ -8006,10 +8003,10 @@
         <v>78</v>
       </c>
       <c r="B131" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C131" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D131" t="s">
         <v>32</v>
@@ -8023,10 +8020,10 @@
         <v>157</v>
       </c>
       <c r="B132" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C132" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D132" t="s">
         <v>32</v>
@@ -8037,13 +8034,13 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B133" t="s">
         <v>78</v>
       </c>
       <c r="C133" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D133" t="s">
         <v>32</v>
@@ -8057,10 +8054,10 @@
         <v>157</v>
       </c>
       <c r="B134" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C134" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D134" t="s">
         <v>32</v>
@@ -8071,13 +8068,13 @@
     </row>
     <row r="135" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B135" t="s">
         <v>176</v>
       </c>
       <c r="C135" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D135" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
work in progress on presentation
</commit_message>
<xml_diff>
--- a/Avengers.xlsx
+++ b/Avengers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Proprietario\Desktop\codici git\avengers ELO rating\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85245FAA-D3EE-4767-8F5B-89D5BCA99954}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBFD2F5-1D44-4980-8408-EAF37BE929C9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{615A6A59-B40D-4CD6-BA71-120B63914EEB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{615A6A59-B40D-4CD6-BA71-120B63914EEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Captain America" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1965" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1965" uniqueCount="288">
   <si>
     <t>winner</t>
   </si>
@@ -428,21 +428,12 @@
     <t>50 caliber jeep</t>
   </si>
   <si>
-    <t>5-Us Army Soldier</t>
-  </si>
-  <si>
     <t>0.1-Hulk</t>
   </si>
   <si>
-    <t>5-Us Army Soldier, 50 caliber jeep</t>
-  </si>
-  <si>
     <t>0.2-Hulk</t>
   </si>
   <si>
-    <t>8-Us Army Soldier</t>
-  </si>
-  <si>
     <t>0.5-Hulk</t>
   </si>
   <si>
@@ -887,22 +878,28 @@
     <t>0.8-Hulk</t>
   </si>
   <si>
-    <t>4-Chitauiri Soldier</t>
-  </si>
-  <si>
     <t>Battaglia di New York - lancio missile nucleare</t>
   </si>
   <si>
     <t>3-Chitauri Soldier</t>
   </si>
   <si>
-    <t>5-Chitauiri Soldier</t>
-  </si>
-  <si>
     <t>Battaglia di New York - Scena Finale</t>
   </si>
   <si>
     <t>Iron Man,Captain America,Thor,Hulk,Black Widow,Hawkeye</t>
+  </si>
+  <si>
+    <t>8-US Army Soldier</t>
+  </si>
+  <si>
+    <t>5-Chitauri Soldier</t>
+  </si>
+  <si>
+    <t>5-US Army Soldier</t>
+  </si>
+  <si>
+    <t>5-US Army Soldier, 50 caliber jeep</t>
   </si>
 </sst>
 </file>
@@ -2351,10 +2348,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B15" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C15" t="s">
         <v>24</v>
@@ -2371,7 +2368,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C16" t="s">
         <v>24</v>
@@ -2631,8 +2628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A6E19BE-BCA4-4601-93CD-8C178C0CE457}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2952,13 +2949,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>286</v>
+      </c>
+      <c r="B19" t="s">
         <v>130</v>
       </c>
-      <c r="B19" t="s">
-        <v>131</v>
-      </c>
       <c r="C19" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D19" t="s">
         <v>32</v>
@@ -2969,13 +2966,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>132</v>
+        <v>287</v>
       </c>
       <c r="B20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C20" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D20" t="s">
         <v>32</v>
@@ -2992,7 +2989,7 @@
         <v>129</v>
       </c>
       <c r="C21" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D21" t="s">
         <v>32</v>
@@ -3009,7 +3006,7 @@
         <v>129</v>
       </c>
       <c r="C22" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D22" t="s">
         <v>32</v>
@@ -3023,10 +3020,10 @@
         <v>111</v>
       </c>
       <c r="B23" t="s">
-        <v>134</v>
+        <v>284</v>
       </c>
       <c r="C23" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D23" t="s">
         <v>32</v>
@@ -3043,7 +3040,7 @@
         <v>125</v>
       </c>
       <c r="C24" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D24" t="s">
         <v>32</v>
@@ -3057,10 +3054,10 @@
         <v>121</v>
       </c>
       <c r="B25" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C25" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D25" t="s">
         <v>32</v>
@@ -3074,10 +3071,10 @@
         <v>121</v>
       </c>
       <c r="B26" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C26" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D26" t="s">
         <v>32</v>
@@ -3091,10 +3088,10 @@
         <v>121</v>
       </c>
       <c r="B27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C27" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D27" t="s">
         <v>32</v>
@@ -3105,13 +3102,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B28" t="s">
         <v>121</v>
       </c>
       <c r="C28" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D28" t="s">
         <v>32</v>
@@ -3122,13 +3119,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B29" t="s">
         <v>111</v>
       </c>
       <c r="C29" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D29" t="s">
         <v>32</v>
@@ -3142,10 +3139,10 @@
         <v>111</v>
       </c>
       <c r="B30" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" t="s">
         <v>137</v>
-      </c>
-      <c r="C30" t="s">
-        <v>140</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -3159,10 +3156,10 @@
         <v>111</v>
       </c>
       <c r="B31" t="s">
+        <v>134</v>
+      </c>
+      <c r="C31" t="s">
         <v>137</v>
-      </c>
-      <c r="C31" t="s">
-        <v>140</v>
       </c>
       <c r="D31" t="s">
         <v>32</v>
@@ -3179,7 +3176,7 @@
         <v>121</v>
       </c>
       <c r="C32" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D32" t="s">
         <v>32</v>
@@ -3190,13 +3187,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>135</v>
+      </c>
+      <c r="B33" t="s">
+        <v>131</v>
+      </c>
+      <c r="C33" t="s">
         <v>138</v>
-      </c>
-      <c r="B33" t="s">
-        <v>133</v>
-      </c>
-      <c r="C33" t="s">
-        <v>141</v>
       </c>
       <c r="D33" t="s">
         <v>33</v>
@@ -3210,10 +3207,10 @@
         <v>111</v>
       </c>
       <c r="B34" t="s">
+        <v>135</v>
+      </c>
+      <c r="C34" t="s">
         <v>138</v>
-      </c>
-      <c r="C34" t="s">
-        <v>141</v>
       </c>
       <c r="D34" t="s">
         <v>32</v>
@@ -3230,7 +3227,7 @@
         <v>124</v>
       </c>
       <c r="C35" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D35" t="s">
         <v>32</v>
@@ -3247,7 +3244,7 @@
         <v>113</v>
       </c>
       <c r="C36" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D36" t="s">
         <v>32</v>
@@ -3264,7 +3261,7 @@
         <v>76</v>
       </c>
       <c r="C37" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D37" t="s">
         <v>32</v>
@@ -3278,10 +3275,10 @@
         <v>121</v>
       </c>
       <c r="B38" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C38" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D38" t="s">
         <v>32</v>
@@ -3292,13 +3289,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B39" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C39" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D39" t="s">
         <v>32</v>
@@ -3309,13 +3306,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B40" t="s">
         <v>45</v>
       </c>
       <c r="C40" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D40" t="s">
         <v>32</v>
@@ -3326,13 +3323,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B41" t="s">
         <v>76</v>
       </c>
       <c r="C41" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D41" t="s">
         <v>32</v>
@@ -3343,13 +3340,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B42" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C42" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D42" t="s">
         <v>32</v>
@@ -3360,13 +3357,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B43" t="s">
         <v>45</v>
       </c>
       <c r="C43" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D43" t="s">
         <v>32</v>
@@ -3377,13 +3374,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B44" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C44" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D44" t="s">
         <v>32</v>
@@ -3394,13 +3391,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B45" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C45" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D45" t="s">
         <v>32</v>
@@ -3411,13 +3408,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B46" t="s">
         <v>7</v>
       </c>
       <c r="C46" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D46" t="s">
         <v>32</v>
@@ -3428,13 +3425,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>142</v>
+      </c>
+      <c r="B47" t="s">
         <v>145</v>
       </c>
-      <c r="B47" t="s">
-        <v>148</v>
-      </c>
       <c r="C47" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D47" t="s">
         <v>32</v>
@@ -3445,13 +3442,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B48" t="s">
+        <v>146</v>
+      </c>
+      <c r="C48" t="s">
         <v>149</v>
-      </c>
-      <c r="C48" t="s">
-        <v>152</v>
       </c>
       <c r="D48" t="s">
         <v>32</v>
@@ -3462,13 +3459,13 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B49" t="s">
         <v>19</v>
       </c>
       <c r="C49" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D49" t="s">
         <v>32</v>
@@ -3479,13 +3476,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B50" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C50" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D50" t="s">
         <v>32</v>
@@ -3496,13 +3493,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B51" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C51" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D51" t="s">
         <v>32</v>
@@ -3513,13 +3510,13 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B52" t="s">
         <v>69</v>
       </c>
       <c r="C52" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D52" t="s">
         <v>32</v>
@@ -3530,13 +3527,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B53" t="s">
         <v>45</v>
       </c>
       <c r="C53" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D53" t="s">
         <v>32</v>
@@ -3547,13 +3544,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B54" t="s">
         <v>18</v>
       </c>
       <c r="C54" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D54" t="s">
         <v>32</v>
@@ -3564,13 +3561,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B55" t="s">
         <v>111</v>
       </c>
       <c r="C55" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D55" t="s">
         <v>32</v>
@@ -3584,10 +3581,10 @@
         <v>111</v>
       </c>
       <c r="B56" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C56" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D56" t="s">
         <v>32</v>
@@ -3601,10 +3598,10 @@
         <v>111</v>
       </c>
       <c r="B57" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C57" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D57" t="s">
         <v>32</v>
@@ -3615,13 +3612,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B58" t="s">
         <v>111</v>
       </c>
       <c r="C58" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D58" t="s">
         <v>32</v>
@@ -3632,13 +3629,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B59" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C59" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D59" t="s">
         <v>33</v>
@@ -3649,13 +3646,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B60" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C60" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D60" t="s">
         <v>33</v>
@@ -3666,13 +3663,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B61" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C61" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D61" t="s">
         <v>32</v>
@@ -3686,10 +3683,10 @@
         <v>111</v>
       </c>
       <c r="B62" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C62" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D62" t="s">
         <v>32</v>
@@ -3700,13 +3697,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B63" t="s">
         <v>111</v>
       </c>
       <c r="C63" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D63" t="s">
         <v>32</v>
@@ -3717,13 +3714,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B64" t="s">
         <v>111</v>
       </c>
       <c r="C64" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D64" t="s">
         <v>32</v>
@@ -3737,10 +3734,10 @@
         <v>111</v>
       </c>
       <c r="B65" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C65" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D65" t="s">
         <v>32</v>
@@ -3759,7 +3756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86623F91-13E1-4965-971C-80C3CB3164C6}">
   <dimension ref="A1:E90"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
+    <sheetView topLeftCell="A66" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -3791,13 +3788,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D2" t="s">
         <v>32</v>
@@ -3808,13 +3805,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D3" t="s">
         <v>32</v>
@@ -3825,13 +3822,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D4" t="s">
         <v>32</v>
@@ -3842,13 +3839,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" t="s">
         <v>159</v>
       </c>
-      <c r="B5" t="s">
-        <v>162</v>
-      </c>
       <c r="C5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D5" t="s">
         <v>32</v>
@@ -3859,13 +3856,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C6" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D6" t="s">
         <v>32</v>
@@ -3876,13 +3873,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B7" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D7" t="s">
         <v>32</v>
@@ -3893,13 +3890,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C8" t="s">
         <v>165</v>
-      </c>
-      <c r="C8" t="s">
-        <v>168</v>
       </c>
       <c r="D8" t="s">
         <v>32</v>
@@ -3910,13 +3907,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C9" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D9" t="s">
         <v>32</v>
@@ -3927,13 +3924,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B10" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C10" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D10" t="s">
         <v>32</v>
@@ -3944,13 +3941,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B11" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C11" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D11" t="s">
         <v>32</v>
@@ -3961,13 +3958,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B12" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C12" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D12" t="s">
         <v>32</v>
@@ -3978,13 +3975,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B13" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C13" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D13" t="s">
         <v>32</v>
@@ -3995,13 +3992,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B14" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C14" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D14" t="s">
         <v>32</v>
@@ -4012,13 +4009,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B15" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C15" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D15" t="s">
         <v>32</v>
@@ -4029,13 +4026,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B16" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C16" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D16" t="s">
         <v>32</v>
@@ -4046,13 +4043,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B17" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C17" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D17" t="s">
         <v>32</v>
@@ -4063,13 +4060,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B18" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C18" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D18" t="s">
         <v>32</v>
@@ -4080,13 +4077,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B19" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C19" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D19" t="s">
         <v>32</v>
@@ -4097,13 +4094,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B20" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C20" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D20" t="s">
         <v>32</v>
@@ -4114,13 +4111,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B21" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C21" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D21" t="s">
         <v>32</v>
@@ -4131,13 +4128,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B22" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C22" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D22" t="s">
         <v>32</v>
@@ -4148,13 +4145,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B23" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C23" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D23" t="s">
         <v>32</v>
@@ -4165,13 +4162,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B24" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C24" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D24" t="s">
         <v>32</v>
@@ -4182,13 +4179,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B25" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C25" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D25" t="s">
         <v>32</v>
@@ -4199,13 +4196,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B26" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C26" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D26" t="s">
         <v>32</v>
@@ -4216,13 +4213,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B27" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D27" t="s">
         <v>32</v>
@@ -4233,13 +4230,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B28" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C28" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D28" t="s">
         <v>32</v>
@@ -4250,13 +4247,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B29" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C29" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D29" t="s">
         <v>32</v>
@@ -4267,13 +4264,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B30" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C30" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -4284,13 +4281,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B31" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C31" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D31" t="s">
         <v>32</v>
@@ -4301,13 +4298,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B32" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C32" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D32" t="s">
         <v>32</v>
@@ -4318,13 +4315,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B33" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C33" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D33" t="s">
         <v>32</v>
@@ -4335,13 +4332,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B34" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C34" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D34" t="s">
         <v>32</v>
@@ -4352,13 +4349,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B35" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C35" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D35" t="s">
         <v>32</v>
@@ -4369,13 +4366,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B36" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C36" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D36" t="s">
         <v>32</v>
@@ -4386,13 +4383,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B37" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C37" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D37" t="s">
         <v>32</v>
@@ -4403,13 +4400,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B38" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C38" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D38" t="s">
         <v>32</v>
@@ -4420,13 +4417,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B39" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C39" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D39" t="s">
         <v>33</v>
@@ -4437,13 +4434,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B40" t="s">
+        <v>182</v>
+      </c>
+      <c r="C40" t="s">
         <v>185</v>
-      </c>
-      <c r="C40" t="s">
-        <v>188</v>
       </c>
       <c r="D40" t="s">
         <v>32</v>
@@ -4454,13 +4451,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B41" t="s">
+        <v>183</v>
+      </c>
+      <c r="C41" t="s">
         <v>186</v>
-      </c>
-      <c r="C41" t="s">
-        <v>189</v>
       </c>
       <c r="D41" t="s">
         <v>32</v>
@@ -4471,13 +4468,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B42" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C42" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D42" t="s">
         <v>32</v>
@@ -4488,13 +4485,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B43" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C43" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D43" t="s">
         <v>32</v>
@@ -4505,13 +4502,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B44" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C44" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D44" t="s">
         <v>32</v>
@@ -4522,13 +4519,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B45" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C45" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D45" t="s">
         <v>32</v>
@@ -4539,13 +4536,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B46" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C46" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D46" t="s">
         <v>32</v>
@@ -4556,13 +4553,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B47" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C47" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D47" t="s">
         <v>33</v>
@@ -4573,13 +4570,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B48" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C48" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D48" t="s">
         <v>32</v>
@@ -4590,13 +4587,13 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B49" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C49" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D49" t="s">
         <v>32</v>
@@ -4607,13 +4604,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B50" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C50" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D50" t="s">
         <v>32</v>
@@ -4624,13 +4621,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B51" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C51" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D51" t="s">
         <v>32</v>
@@ -4641,13 +4638,13 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B52" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C52" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D52" t="s">
         <v>32</v>
@@ -4658,13 +4655,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B53" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C53" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D53" t="s">
         <v>32</v>
@@ -4675,13 +4672,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B54" t="s">
         <v>108</v>
       </c>
       <c r="C54" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D54" t="s">
         <v>32</v>
@@ -4692,13 +4689,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B55" t="s">
         <v>108</v>
       </c>
       <c r="C55" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D55" t="s">
         <v>32</v>
@@ -4709,13 +4706,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B56" t="s">
         <v>17</v>
       </c>
       <c r="C56" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D56" t="s">
         <v>32</v>
@@ -4726,13 +4723,13 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B57" t="s">
         <v>17</v>
       </c>
       <c r="C57" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D57" t="s">
         <v>32</v>
@@ -4743,13 +4740,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B58" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C58" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D58" t="s">
         <v>32</v>
@@ -4760,13 +4757,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B59" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C59" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D59" t="s">
         <v>32</v>
@@ -4777,13 +4774,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B60" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C60" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D60" t="s">
         <v>32</v>
@@ -4794,13 +4791,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B61" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C61" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D61" t="s">
         <v>32</v>
@@ -4811,13 +4808,13 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B62" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C62" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D62" t="s">
         <v>32</v>
@@ -4828,13 +4825,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B63" t="s">
         <v>19</v>
       </c>
       <c r="C63" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D63" t="s">
         <v>32</v>
@@ -4845,13 +4842,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B64" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C64" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D64" t="s">
         <v>32</v>
@@ -4862,13 +4859,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B65" t="s">
         <v>63</v>
       </c>
       <c r="C65" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D65" t="s">
         <v>32</v>
@@ -4879,13 +4876,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B66" t="s">
         <v>19</v>
       </c>
       <c r="C66" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D66" t="s">
         <v>32</v>
@@ -4896,13 +4893,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B67" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C67" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D67" t="s">
         <v>32</v>
@@ -4913,13 +4910,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B68" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C68" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D68" t="s">
         <v>32</v>
@@ -4930,13 +4927,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B69" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C69" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D69" t="s">
         <v>32</v>
@@ -4947,13 +4944,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B70" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C70" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D70" t="s">
         <v>32</v>
@@ -4964,13 +4961,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B71" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C71" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D71" t="s">
         <v>32</v>
@@ -4981,13 +4978,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
+        <v>167</v>
+      </c>
+      <c r="B72" t="s">
         <v>170</v>
       </c>
-      <c r="B72" t="s">
-        <v>173</v>
-      </c>
       <c r="C72" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D72" t="s">
         <v>32</v>
@@ -4998,13 +4995,13 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B73" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C73" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D73" t="s">
         <v>32</v>
@@ -5015,13 +5012,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B74" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C74" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D74" t="s">
         <v>32</v>
@@ -5032,13 +5029,13 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B75" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C75" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D75" t="s">
         <v>32</v>
@@ -5049,13 +5046,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B76" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C76" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D76" t="s">
         <v>32</v>
@@ -5066,13 +5063,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B77" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C77" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D77" t="s">
         <v>32</v>
@@ -5083,13 +5080,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B78" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C78" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D78" t="s">
         <v>33</v>
@@ -5100,13 +5097,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B79" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C79" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D79" t="s">
         <v>32</v>
@@ -5117,13 +5114,13 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B80" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C80" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D80" t="s">
         <v>32</v>
@@ -5134,13 +5131,13 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B81" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C81" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D81" t="s">
         <v>32</v>
@@ -5151,13 +5148,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B82" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C82" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D82" t="s">
         <v>32</v>
@@ -5168,13 +5165,13 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B83" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C83" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D83" t="s">
         <v>32</v>
@@ -5185,13 +5182,13 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B84" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C84" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D84" t="s">
         <v>32</v>
@@ -5202,13 +5199,13 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B85" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C85" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D85" t="s">
         <v>32</v>
@@ -5219,13 +5216,13 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B86" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C86" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D86" t="s">
         <v>32</v>
@@ -5236,13 +5233,13 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B87" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C87" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D87" t="s">
         <v>32</v>
@@ -5253,13 +5250,13 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B88" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C88" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D88" t="s">
         <v>32</v>
@@ -5270,13 +5267,13 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B89" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C89" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D89" t="s">
         <v>32</v>
@@ -5287,13 +5284,13 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B90" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C90" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D90" t="s">
         <v>32</v>
@@ -5311,7 +5308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97203B1C-8A29-4438-986F-111AFC7E55B4}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -5775,8 +5772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21457546-0B28-49FC-B4FE-8AD5E29F1C13}">
   <dimension ref="A1:E135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView topLeftCell="A114" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A133" sqref="A133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5807,13 +5804,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D2" t="s">
         <v>32</v>
@@ -5824,13 +5821,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D3" t="s">
         <v>32</v>
@@ -5841,13 +5838,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B4" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D4" t="s">
         <v>32</v>
@@ -5858,13 +5855,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D5" t="s">
         <v>32</v>
@@ -5875,13 +5872,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B6" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C6" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D6" t="s">
         <v>32</v>
@@ -5892,13 +5889,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D7" t="s">
         <v>32</v>
@@ -5909,13 +5906,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B8" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C8" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D8" t="s">
         <v>32</v>
@@ -5926,13 +5923,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B9" t="s">
         <v>108</v>
       </c>
       <c r="C9" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D9" t="s">
         <v>32</v>
@@ -5943,13 +5940,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B10" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C10" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D10" t="s">
         <v>32</v>
@@ -5960,13 +5957,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B11" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C11" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D11" t="s">
         <v>32</v>
@@ -5980,10 +5977,10 @@
         <v>48</v>
       </c>
       <c r="B12" t="s">
+        <v>218</v>
+      </c>
+      <c r="C12" t="s">
         <v>221</v>
-      </c>
-      <c r="C12" t="s">
-        <v>224</v>
       </c>
       <c r="D12" t="s">
         <v>32</v>
@@ -5997,10 +5994,10 @@
         <v>48</v>
       </c>
       <c r="B13" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C13" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D13" t="s">
         <v>32</v>
@@ -6011,13 +6008,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B14" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C14" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D14" t="s">
         <v>32</v>
@@ -6028,13 +6025,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B15" t="s">
         <v>117</v>
       </c>
       <c r="C15" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D15" t="s">
         <v>32</v>
@@ -6045,13 +6042,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B16" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C16" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D16" t="s">
         <v>32</v>
@@ -6062,13 +6059,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B17" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C17" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D17" t="s">
         <v>32</v>
@@ -6082,10 +6079,10 @@
         <v>78</v>
       </c>
       <c r="B18" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C18" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D18" t="s">
         <v>32</v>
@@ -6096,13 +6093,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B19" t="s">
         <v>78</v>
       </c>
       <c r="C19" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D19" t="s">
         <v>32</v>
@@ -6116,10 +6113,10 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C20" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D20" t="s">
         <v>33</v>
@@ -6130,13 +6127,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B21" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C21" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D21" t="s">
         <v>32</v>
@@ -6147,13 +6144,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B22" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C22" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D22" t="s">
         <v>32</v>
@@ -6167,10 +6164,10 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C23" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D23" t="s">
         <v>33</v>
@@ -6181,13 +6178,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B24" t="s">
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D24" t="s">
         <v>32</v>
@@ -6201,10 +6198,10 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C25" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D25" t="s">
         <v>32</v>
@@ -6215,13 +6212,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B26" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C26" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D26" t="s">
         <v>32</v>
@@ -6235,10 +6232,10 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C27" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D27" t="s">
         <v>32</v>
@@ -6249,13 +6246,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B28" t="s">
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D28" t="s">
         <v>32</v>
@@ -6266,13 +6263,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B29" t="s">
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D29" t="s">
         <v>32</v>
@@ -6286,10 +6283,10 @@
         <v>78</v>
       </c>
       <c r="B30" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C30" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -6306,7 +6303,7 @@
         <v>48</v>
       </c>
       <c r="C31" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D31" t="s">
         <v>32</v>
@@ -6317,13 +6314,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B32" t="s">
         <v>111</v>
       </c>
       <c r="C32" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D32" t="s">
         <v>32</v>
@@ -6334,13 +6331,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B33" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C33" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D33" t="s">
         <v>32</v>
@@ -6354,10 +6351,10 @@
         <v>111</v>
       </c>
       <c r="B34" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C34" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D34" t="s">
         <v>32</v>
@@ -6368,13 +6365,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B35" t="s">
         <v>111</v>
       </c>
       <c r="C35" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D35" t="s">
         <v>32</v>
@@ -6385,13 +6382,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B36" t="s">
         <v>111</v>
       </c>
       <c r="C36" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D36" t="s">
         <v>32</v>
@@ -6402,13 +6399,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B37" t="s">
         <v>108</v>
       </c>
       <c r="C37" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D37" t="s">
         <v>32</v>
@@ -6419,13 +6416,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B38" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C38" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D38" t="s">
         <v>32</v>
@@ -6436,13 +6433,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B39" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C39" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D39" t="s">
         <v>32</v>
@@ -6453,13 +6450,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B40" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C40" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D40" t="s">
         <v>32</v>
@@ -6470,13 +6467,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B41" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C41" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D41" t="s">
         <v>32</v>
@@ -6487,13 +6484,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B42" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C42" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D42" t="s">
         <v>33</v>
@@ -6507,10 +6504,10 @@
         <v>111</v>
       </c>
       <c r="B43" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C43" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D43" t="s">
         <v>33</v>
@@ -6524,10 +6521,10 @@
         <v>78</v>
       </c>
       <c r="B44" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C44" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D44" t="s">
         <v>32</v>
@@ -6538,13 +6535,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B45" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C45" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D45" t="s">
         <v>32</v>
@@ -6555,13 +6552,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B46" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C46" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D46" t="s">
         <v>32</v>
@@ -6572,13 +6569,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B47" t="s">
         <v>78</v>
       </c>
       <c r="C47" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D47" t="s">
         <v>32</v>
@@ -6589,13 +6586,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B48" t="s">
+        <v>239</v>
+      </c>
+      <c r="C48" t="s">
         <v>242</v>
-      </c>
-      <c r="C48" t="s">
-        <v>245</v>
       </c>
       <c r="D48" t="s">
         <v>32</v>
@@ -6609,10 +6606,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C49" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D49" t="s">
         <v>32</v>
@@ -6626,10 +6623,10 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C50" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D50" t="s">
         <v>32</v>
@@ -6643,10 +6640,10 @@
         <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C51" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D51" t="s">
         <v>32</v>
@@ -6660,10 +6657,10 @@
         <v>63</v>
       </c>
       <c r="B52" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C52" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D52" t="s">
         <v>32</v>
@@ -6674,13 +6671,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B53" t="s">
         <v>63</v>
       </c>
       <c r="C53" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D53" t="s">
         <v>32</v>
@@ -6694,10 +6691,10 @@
         <v>48</v>
       </c>
       <c r="B54" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C54" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D54" t="s">
         <v>32</v>
@@ -6711,10 +6708,10 @@
         <v>48</v>
       </c>
       <c r="B55" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C55" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D55" t="s">
         <v>32</v>
@@ -6728,10 +6725,10 @@
         <v>63</v>
       </c>
       <c r="B56" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C56" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D56" t="s">
         <v>32</v>
@@ -6745,10 +6742,10 @@
         <v>2</v>
       </c>
       <c r="B57" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C57" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D57" t="s">
         <v>33</v>
@@ -6762,10 +6759,10 @@
         <v>38</v>
       </c>
       <c r="B58" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C58" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D58" t="s">
         <v>32</v>
@@ -6776,13 +6773,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B59" t="s">
         <v>38</v>
       </c>
       <c r="C59" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D59" t="s">
         <v>32</v>
@@ -6796,10 +6793,10 @@
         <v>2</v>
       </c>
       <c r="B60" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C60" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D60" t="s">
         <v>33</v>
@@ -6813,10 +6810,10 @@
         <v>2</v>
       </c>
       <c r="B61" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C61" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D61" t="s">
         <v>33</v>
@@ -6830,10 +6827,10 @@
         <v>2</v>
       </c>
       <c r="B62" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C62" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D62" t="s">
         <v>33</v>
@@ -6844,13 +6841,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B63" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C63" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D63" t="s">
         <v>33</v>
@@ -6861,13 +6858,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B64" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C64" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D64" t="s">
         <v>33</v>
@@ -6878,13 +6875,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B65" t="s">
         <v>19</v>
       </c>
       <c r="C65" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D65" t="s">
         <v>33</v>
@@ -6898,10 +6895,10 @@
         <v>2</v>
       </c>
       <c r="B66" t="s">
+        <v>253</v>
+      </c>
+      <c r="C66" t="s">
         <v>256</v>
-      </c>
-      <c r="C66" t="s">
-        <v>259</v>
       </c>
       <c r="D66" t="s">
         <v>33</v>
@@ -6912,13 +6909,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B67" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C67" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D67" t="s">
         <v>33</v>
@@ -6929,13 +6926,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B68" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C68" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D68" t="s">
         <v>33</v>
@@ -6946,13 +6943,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B69" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C69" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D69" t="s">
         <v>32</v>
@@ -6963,13 +6960,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B70" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C70" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D70" t="s">
         <v>32</v>
@@ -6980,13 +6977,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B71" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C71" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D71" t="s">
         <v>32</v>
@@ -6997,13 +6994,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B72" t="s">
         <v>18</v>
       </c>
       <c r="C72" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D72" t="s">
         <v>32</v>
@@ -7014,13 +7011,13 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B73" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C73" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D73" t="s">
         <v>32</v>
@@ -7031,13 +7028,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B74" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C74" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D74" t="s">
         <v>32</v>
@@ -7048,13 +7045,13 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B75" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C75" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D75" t="s">
         <v>32</v>
@@ -7065,13 +7062,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
+        <v>259</v>
+      </c>
+      <c r="B76" t="s">
         <v>262</v>
       </c>
-      <c r="B76" t="s">
-        <v>265</v>
-      </c>
       <c r="C76" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D76" t="s">
         <v>32</v>
@@ -7082,13 +7079,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B77" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C77" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D77" t="s">
         <v>32</v>
@@ -7102,10 +7099,10 @@
         <v>48</v>
       </c>
       <c r="B78" t="s">
+        <v>258</v>
+      </c>
+      <c r="C78" t="s">
         <v>261</v>
-      </c>
-      <c r="C78" t="s">
-        <v>264</v>
       </c>
       <c r="D78" t="s">
         <v>32</v>
@@ -7119,10 +7116,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C79" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D79" t="s">
         <v>32</v>
@@ -7133,13 +7130,13 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B80" t="s">
+        <v>258</v>
+      </c>
+      <c r="C80" t="s">
         <v>261</v>
-      </c>
-      <c r="C80" t="s">
-        <v>264</v>
       </c>
       <c r="D80" t="s">
         <v>32</v>
@@ -7153,10 +7150,10 @@
         <v>48</v>
       </c>
       <c r="B81" t="s">
+        <v>258</v>
+      </c>
+      <c r="C81" t="s">
         <v>261</v>
-      </c>
-      <c r="C81" t="s">
-        <v>264</v>
       </c>
       <c r="D81" t="s">
         <v>32</v>
@@ -7167,13 +7164,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
+        <v>258</v>
+      </c>
+      <c r="B82" t="s">
+        <v>211</v>
+      </c>
+      <c r="C82" t="s">
         <v>261</v>
-      </c>
-      <c r="B82" t="s">
-        <v>214</v>
-      </c>
-      <c r="C82" t="s">
-        <v>264</v>
       </c>
       <c r="D82" t="s">
         <v>32</v>
@@ -7187,10 +7184,10 @@
         <v>48</v>
       </c>
       <c r="B83" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C83" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D83" t="s">
         <v>32</v>
@@ -7201,13 +7198,13 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B84" t="s">
+        <v>258</v>
+      </c>
+      <c r="C84" t="s">
         <v>261</v>
-      </c>
-      <c r="C84" t="s">
-        <v>264</v>
       </c>
       <c r="D84" t="s">
         <v>32</v>
@@ -7218,13 +7215,13 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B85" t="s">
+        <v>258</v>
+      </c>
+      <c r="C85" t="s">
         <v>261</v>
-      </c>
-      <c r="C85" t="s">
-        <v>264</v>
       </c>
       <c r="D85" t="s">
         <v>32</v>
@@ -7238,10 +7235,10 @@
         <v>78</v>
       </c>
       <c r="B86" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C86" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D86" t="s">
         <v>32</v>
@@ -7252,13 +7249,13 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B87" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C87" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D87" t="s">
         <v>33</v>
@@ -7269,13 +7266,13 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B88" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C88" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D88" t="s">
         <v>32</v>
@@ -7289,10 +7286,10 @@
         <v>111</v>
       </c>
       <c r="B89" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C89" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D89" t="s">
         <v>33</v>
@@ -7306,10 +7303,10 @@
         <v>111</v>
       </c>
       <c r="B90" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C90" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D90" t="s">
         <v>33</v>
@@ -7320,13 +7317,13 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B91" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C91" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D91" t="s">
         <v>32</v>
@@ -7337,13 +7334,13 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B92" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C92" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D92" t="s">
         <v>32</v>
@@ -7354,13 +7351,13 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B93" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C93" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D93" t="s">
         <v>32</v>
@@ -7374,10 +7371,10 @@
         <v>2</v>
       </c>
       <c r="B94" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C94" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D94" t="s">
         <v>33</v>
@@ -7391,10 +7388,10 @@
         <v>2</v>
       </c>
       <c r="B95" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C95" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D95" t="s">
         <v>33</v>
@@ -7405,13 +7402,13 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B96" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C96" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D96" t="s">
         <v>32</v>
@@ -7425,10 +7422,10 @@
         <v>48</v>
       </c>
       <c r="B97" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C97" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D97" t="s">
         <v>32</v>
@@ -7442,10 +7439,10 @@
         <v>48</v>
       </c>
       <c r="B98" t="s">
+        <v>264</v>
+      </c>
+      <c r="C98" t="s">
         <v>267</v>
-      </c>
-      <c r="C98" t="s">
-        <v>270</v>
       </c>
       <c r="D98" t="s">
         <v>33</v>
@@ -7459,10 +7456,10 @@
         <v>2</v>
       </c>
       <c r="B99" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C99" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D99" t="s">
         <v>33</v>
@@ -7476,10 +7473,10 @@
         <v>2</v>
       </c>
       <c r="B100" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C100" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D100" t="s">
         <v>33</v>
@@ -7493,10 +7490,10 @@
         <v>78</v>
       </c>
       <c r="B101" t="s">
+        <v>264</v>
+      </c>
+      <c r="C101" t="s">
         <v>267</v>
-      </c>
-      <c r="C101" t="s">
-        <v>270</v>
       </c>
       <c r="D101" t="s">
         <v>32</v>
@@ -7510,10 +7507,10 @@
         <v>2</v>
       </c>
       <c r="B102" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C102" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D102" t="s">
         <v>32</v>
@@ -7524,13 +7521,13 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B103" t="s">
+        <v>264</v>
+      </c>
+      <c r="C103" t="s">
         <v>267</v>
-      </c>
-      <c r="C103" t="s">
-        <v>270</v>
       </c>
       <c r="D103" t="s">
         <v>32</v>
@@ -7544,10 +7541,10 @@
         <v>2</v>
       </c>
       <c r="B104" t="s">
+        <v>264</v>
+      </c>
+      <c r="C104" t="s">
         <v>267</v>
-      </c>
-      <c r="C104" t="s">
-        <v>270</v>
       </c>
       <c r="D104" t="s">
         <v>33</v>
@@ -7558,13 +7555,13 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B105" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C105" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D105" t="s">
         <v>32</v>
@@ -7575,13 +7572,13 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B106" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C106" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D106" t="s">
         <v>32</v>
@@ -7595,10 +7592,10 @@
         <v>111</v>
       </c>
       <c r="B107" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C107" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D107" t="s">
         <v>32</v>
@@ -7609,13 +7606,13 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B108" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C108" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D108" t="s">
         <v>32</v>
@@ -7626,13 +7623,13 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B109" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C109" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D109" t="s">
         <v>32</v>
@@ -7646,10 +7643,10 @@
         <v>111</v>
       </c>
       <c r="B110" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C110" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D110" t="s">
         <v>32</v>
@@ -7660,13 +7657,13 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B111" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C111" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D111" t="s">
         <v>32</v>
@@ -7680,10 +7677,10 @@
         <v>78</v>
       </c>
       <c r="B112" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C112" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D112" t="s">
         <v>32</v>
@@ -7697,10 +7694,10 @@
         <v>78</v>
       </c>
       <c r="B113" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C113" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D113" t="s">
         <v>32</v>
@@ -7711,13 +7708,13 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B114" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C114" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D114" t="s">
         <v>32</v>
@@ -7731,10 +7728,10 @@
         <v>78</v>
       </c>
       <c r="B115" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C115" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D115" t="s">
         <v>32</v>
@@ -7745,13 +7742,13 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B116" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C116" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D116" t="s">
         <v>32</v>
@@ -7762,13 +7759,13 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B117" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C117" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D117" t="s">
         <v>32</v>
@@ -7782,10 +7779,10 @@
         <v>111</v>
       </c>
       <c r="B118" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C118" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D118" t="s">
         <v>33</v>
@@ -7799,10 +7796,10 @@
         <v>111</v>
       </c>
       <c r="B119" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C119" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D119" t="s">
         <v>32</v>
@@ -7816,10 +7813,10 @@
         <v>111</v>
       </c>
       <c r="B120" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C120" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D120" t="s">
         <v>32</v>
@@ -7830,13 +7827,13 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B121" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C121" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D121" t="s">
         <v>33</v>
@@ -7847,13 +7844,13 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B122" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C122" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D122" t="s">
         <v>33</v>
@@ -7867,10 +7864,10 @@
         <v>2</v>
       </c>
       <c r="B123" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C123" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D123" t="s">
         <v>33</v>
@@ -7881,13 +7878,13 @@
     </row>
     <row r="124" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B124" t="s">
         <v>2</v>
       </c>
       <c r="C124" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D124" t="s">
         <v>32</v>
@@ -7898,13 +7895,13 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B125" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C125" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D125" t="s">
         <v>32</v>
@@ -7918,10 +7915,10 @@
         <v>111</v>
       </c>
       <c r="B126" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C126" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D126" t="s">
         <v>32</v>
@@ -7932,13 +7929,13 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B127" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C127" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D127" t="s">
         <v>33</v>
@@ -7949,13 +7946,13 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B128" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C128" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D128" t="s">
         <v>32</v>
@@ -7966,13 +7963,13 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B129" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C129" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D129" t="s">
         <v>32</v>
@@ -7986,10 +7983,10 @@
         <v>2</v>
       </c>
       <c r="B130" t="s">
-        <v>283</v>
+        <v>263</v>
       </c>
       <c r="C130" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D130" t="s">
         <v>32</v>
@@ -8003,10 +8000,10 @@
         <v>78</v>
       </c>
       <c r="B131" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C131" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D131" t="s">
         <v>32</v>
@@ -8017,13 +8014,13 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B132" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C132" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D132" t="s">
         <v>32</v>
@@ -8034,13 +8031,13 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B133" t="s">
         <v>78</v>
       </c>
       <c r="C133" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D133" t="s">
         <v>32</v>
@@ -8051,13 +8048,13 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B134" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C134" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D134" t="s">
         <v>32</v>
@@ -8068,13 +8065,13 @@
     </row>
     <row r="135" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B135" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C135" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="D135" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
work in progress on presentation 3
</commit_message>
<xml_diff>
--- a/Avengers.xlsx
+++ b/Avengers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Proprietario\Desktop\codici git\avengers ELO rating\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2ACDFE3-BBEB-4905-B232-4F18A8A48FE3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA19ECE-4B7B-43C5-92C9-5A205A265678}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{615A6A59-B40D-4CD6-BA71-120B63914EEB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{615A6A59-B40D-4CD6-BA71-120B63914EEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Captain America" sheetId="3" r:id="rId1"/>
@@ -896,10 +896,10 @@
     <t>5-US Army Soldier</t>
   </si>
   <si>
-    <t>5-US Army Soldier, 50 caliber jeep</t>
-  </si>
-  <si>
     <t>Iron Man,Pepper Potts</t>
+  </si>
+  <si>
+    <t>5-US Army Soldier,50 caliber jeep</t>
   </si>
 </sst>
 </file>
@@ -2603,7 +2603,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>14</v>
@@ -2628,8 +2628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A6E19BE-BCA4-4601-93CD-8C178C0CE457}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2966,7 +2966,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B20" t="s">
         <v>130</v>
@@ -5308,7 +5308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97203B1C-8A29-4438-986F-111AFC7E55B4}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>